<commit_message>
did a lot of stuff
</commit_message>
<xml_diff>
--- a/losses/results_1.xlsx
+++ b/losses/results_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\School\2018-19\Fall\ME 4900-028        Robotic Agriculture\ag-mech-clemson\losses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90D8CDEB-CDA6-43ED-85A6-45CB6EDAFCEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD90D852-3A29-4DD9-9E18-4269C915B19A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{733ACD6C-D261-4F74-9AC8-E526882B0448}"/>
   </bookViews>
@@ -30,12 +30,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>X AXIS</t>
   </si>
   <si>
     <t>Y AXIS</t>
+  </si>
+  <si>
+    <t>y [in]</t>
   </si>
 </sst>
 </file>
@@ -88,6 +91,1895 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X AXIS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8298</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8410</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8357</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8720</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8447</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8485</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8320</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8317</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8421</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8314</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8326</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8489</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8375</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8335</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8325</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ABDD-480E-8FA5-F633116A4968}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="374007584"/>
+        <c:axId val="320046368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="374007584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="320046368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="320046368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374007584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y AXIS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3344</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3343</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E27-4D03-89A2-C2CEA7FCB94F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="374467216"/>
+        <c:axId val="315164816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="374467216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="315164816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="315164816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374467216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{329347E5-3349-4BC4-9842-E3DCA5B97F05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F1FBB34-90D6-466C-B753-4BBE7CC901D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,10 +2279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41345359-A794-44B0-9018-7E85EAC8CEB0}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +2415,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8489</v>
       </c>
@@ -531,7 +2423,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8375</v>
       </c>
@@ -539,7 +2431,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8335</v>
       </c>
@@ -547,7 +2439,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8325</v>
       </c>
@@ -555,7 +2447,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8485</v>
       </c>
@@ -563,7 +2455,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>MAX(A2:A21)-MIN(A2:A21)</f>
         <v>432</v>
@@ -573,7 +2465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>_xlfn.STDEV.S(A2:A21)</f>
         <v>102.6155189863702</v>
@@ -583,7 +2475,47 @@
         <v>5.7847349027191255</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>33.5</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <f>C31-C32</f>
+        <v>26.5</v>
+      </c>
+      <c r="D33">
+        <f>D31-D32</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f>C33/AVERAGE($B$2:$B$21)</f>
+        <v>7.9481719204582951E-3</v>
+      </c>
+      <c r="D34">
+        <f>D33/AVERAGE($B$2:$B$21)</f>
+        <v>6.8984133649260676E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>